<commit_message>
check quyền thành công
</commit_message>
<xml_diff>
--- a/ServiceGeneratorTool/DbSchema.xlsx
+++ b/ServiceGeneratorTool/DbSchema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Restaurant\restaurant-management-api\ServiceGeneratorTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EAAD1A-B5C9-456C-B79A-E36C68A0B63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385578E0-4F8F-4F51-BF9D-390933BAB375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5682C2DE-D9BC-4AE6-9095-A6F08CD2E77F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="197">
   <si>
     <t>TableName</t>
   </si>
@@ -120,9 +120,6 @@
     <t>RoleName</t>
   </si>
   <si>
-    <t>UserFunctionIdList</t>
-  </si>
-  <si>
     <t>Tên quyền</t>
   </si>
   <si>
@@ -568,6 +565,57 @@
   </si>
   <si>
     <t>EndTime</t>
+  </si>
+  <si>
+    <t>Token</t>
+  </si>
+  <si>
+    <t>RefreshToken</t>
+  </si>
+  <si>
+    <t>RefreshTokenId</t>
+  </si>
+  <si>
+    <t>ExpiresAt</t>
+  </si>
+  <si>
+    <t>CreatedByIp</t>
+  </si>
+  <si>
+    <t>RevokedAt</t>
+  </si>
+  <si>
+    <t>ReplacedByToken</t>
+  </si>
+  <si>
+    <t>Mã refresh token</t>
+  </si>
+  <si>
+    <t>Chuỗi refresh token</t>
+  </si>
+  <si>
+    <t>Hạn dùng</t>
+  </si>
+  <si>
+    <t>IP đăng nhập</t>
+  </si>
+  <si>
+    <t>Thu hồi chưa</t>
+  </si>
+  <si>
+    <t>Nếu bị thay thì bị thay bởi token nào</t>
+  </si>
+  <si>
+    <t>Token còn hợp lệ không</t>
+  </si>
+  <si>
+    <t>FunctionCode</t>
+  </si>
+  <si>
+    <t>Định danh chức năng</t>
+  </si>
+  <si>
+    <t>FunctionIdList</t>
   </si>
 </sst>
 </file>
@@ -950,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D1BB7ED-A112-494B-BC7C-AC8397CA64F1}">
-  <dimension ref="A1:D126"/>
+  <dimension ref="A1:D136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1081,13 +1129,13 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>132</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1109,32 +1157,32 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>181</v>
       </c>
       <c r="B13" t="s">
-        <v>132</v>
+        <v>182</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>133</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>181</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
@@ -1148,1328 +1196,1454 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>181</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>180</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>134</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>181</v>
       </c>
       <c r="B16" t="s">
-        <v>151</v>
+        <v>183</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>181</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>184</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>181</v>
       </c>
       <c r="B18" t="s">
-        <v>149</v>
+        <v>185</v>
       </c>
       <c r="C18" t="s">
         <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>150</v>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19" t="s">
+        <v>186</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B20" t="s">
-        <v>175</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>11</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>179</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>175</v>
+        <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>150</v>
       </c>
       <c r="C25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>23</v>
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>148</v>
       </c>
       <c r="C27" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" t="s">
-        <v>32</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>175</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>174</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>175</v>
       </c>
       <c r="B30" t="s">
-        <v>164</v>
+        <v>194</v>
       </c>
       <c r="C30" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>165</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" t="s">
-        <v>180</v>
-      </c>
-      <c r="C31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" t="s">
-        <v>166</v>
+      <c r="A31" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" t="s">
-        <v>177</v>
-      </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>174</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
-      <c r="D34" t="s">
-        <v>36</v>
+      <c r="D34" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" t="s">
-        <v>38</v>
+        <v>4</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C37" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
+        <v>196</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>45</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" t="s">
+        <v>163</v>
+      </c>
+      <c r="C40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>179</v>
       </c>
       <c r="C41" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D41" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="B42" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C42" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" t="s">
-        <v>46</v>
-      </c>
-      <c r="B43" t="s">
-        <v>170</v>
-      </c>
-      <c r="C43" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="C44" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="D45" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>71</v>
+        <v>33</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D46" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="D47" t="s">
-        <v>54</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="B49" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C49" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" t="s">
-        <v>55</v>
-      </c>
-      <c r="B50" t="s">
-        <v>47</v>
-      </c>
-      <c r="C50" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B51" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C51" t="s">
         <v>4</v>
       </c>
       <c r="D51" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B52" t="s">
-        <v>58</v>
+        <v>166</v>
       </c>
       <c r="C52" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D52" t="s">
-        <v>59</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B53" t="s">
-        <v>60</v>
+        <v>169</v>
       </c>
       <c r="C53" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="D53" t="s">
-        <v>61</v>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>45</v>
+      </c>
+      <c r="B54" t="s">
+        <v>48</v>
+      </c>
+      <c r="C54" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B55" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C55" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="D55" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>62</v>
-      </c>
-      <c r="B56" t="s">
-        <v>5</v>
+        <v>45</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="C56" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D56" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B57" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C57" t="s">
         <v>6</v>
       </c>
       <c r="D57" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" t="s">
-        <v>62</v>
-      </c>
-      <c r="B58" t="s">
-        <v>39</v>
-      </c>
-      <c r="C58" t="s">
-        <v>40</v>
-      </c>
-      <c r="D58" t="s">
-        <v>66</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>54</v>
+      </c>
+      <c r="B59" t="s">
+        <v>55</v>
+      </c>
+      <c r="C59" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B60" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="C60" t="s">
         <v>4</v>
       </c>
       <c r="D60" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B61" t="s">
+        <v>34</v>
+      </c>
+      <c r="C61" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" t="s">
         <v>35</v>
-      </c>
-      <c r="C61" t="s">
-        <v>4</v>
-      </c>
-      <c r="D61" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B62" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C62" t="s">
         <v>4</v>
       </c>
       <c r="D62" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B63" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C63" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D63" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>78</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>72</v>
+        <v>61</v>
+      </c>
+      <c r="B65" t="s">
+        <v>62</v>
+      </c>
+      <c r="C65" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>78</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>74</v>
+        <v>61</v>
+      </c>
+      <c r="B66" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>78</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>75</v>
+        <v>61</v>
+      </c>
+      <c r="B67" t="s">
+        <v>41</v>
+      </c>
+      <c r="C67" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>78</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" t="s">
-        <v>78</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>163</v>
+        <v>61</v>
+      </c>
+      <c r="B68" t="s">
+        <v>38</v>
+      </c>
+      <c r="C68" t="s">
+        <v>39</v>
+      </c>
+      <c r="D68" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>66</v>
+      </c>
+      <c r="B70" t="s">
+        <v>67</v>
+      </c>
+      <c r="C70" t="s">
+        <v>4</v>
+      </c>
+      <c r="D70" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B71" t="s">
-        <v>80</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>85</v>
+        <v>34</v>
+      </c>
+      <c r="C71" t="s">
+        <v>4</v>
+      </c>
+      <c r="D71" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B72" t="s">
-        <v>97</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>86</v>
+        <v>62</v>
+      </c>
+      <c r="C72" t="s">
+        <v>4</v>
+      </c>
+      <c r="D72" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B73" t="s">
-        <v>81</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" t="s">
-        <v>79</v>
-      </c>
-      <c r="B74" t="s">
-        <v>89</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>90</v>
+        <v>57</v>
+      </c>
+      <c r="C73" t="s">
+        <v>39</v>
+      </c>
+      <c r="D73" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>79</v>
-      </c>
-      <c r="B75" t="s">
-        <v>83</v>
+        <v>77</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
+        <v>77</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
+        <v>77</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" t="s">
+        <v>77</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>77</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" t="s">
+        <v>78</v>
+      </c>
+      <c r="B81" t="s">
         <v>79</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C81" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D81" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D76" s="2" t="s">
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" t="s">
+        <v>78</v>
+      </c>
+      <c r="B82" t="s">
+        <v>96</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" t="s">
+        <v>78</v>
+      </c>
+      <c r="B83" t="s">
+        <v>80</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" t="s">
+        <v>78</v>
+      </c>
+      <c r="B84" t="s">
+        <v>88</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" t="s">
+        <v>78</v>
+      </c>
+      <c r="B85" t="s">
+        <v>82</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" t="s">
+        <v>78</v>
+      </c>
+      <c r="B86" t="s">
+        <v>83</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B88" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B78" t="s">
-        <v>92</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A79" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="A82" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
-      <c r="A83" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B84" t="s">
-        <v>104</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4">
-      <c r="A87" t="s">
-        <v>96</v>
-      </c>
-      <c r="B87" t="s">
-        <v>97</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
-      <c r="A88" t="s">
-        <v>96</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>98</v>
-      </c>
       <c r="C88" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
-      <c r="A89" t="s">
-        <v>96</v>
+    <row r="89" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A89" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>42</v>
+        <v>129</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>103</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B92" t="s">
-        <v>120</v>
+        <v>93</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="4" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>58</v>
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>103</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" t="s">
+        <v>95</v>
+      </c>
+      <c r="B97" t="s">
+        <v>96</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" t="s">
+        <v>95</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" t="s">
+        <v>95</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B101" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B95" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4">
-      <c r="A96" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B96" s="5" t="s">
+      <c r="C101" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B102" t="s">
+        <v>119</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D104" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C96" s="2" t="s">
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C106" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D96" s="2" t="s">
+      <c r="D106" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B107" s="5" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="A97" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B97" s="5" t="s">
+      <c r="C107" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D107" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C97" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D97" s="2" t="s">
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B108" s="5" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="98" spans="1:4">
-      <c r="A98" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B98" s="5" t="s">
+      <c r="C108" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D108" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C98" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D98" s="2" t="s">
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B109" s="5" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="99" spans="1:4">
-      <c r="A99" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B99" s="5" t="s">
+      <c r="C109" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="D109" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" t="s">
-        <v>119</v>
-      </c>
-      <c r="B101" t="s">
-        <v>120</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4">
-      <c r="A102" t="s">
-        <v>119</v>
-      </c>
-      <c r="B102" t="s">
-        <v>5</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4">
-      <c r="A103" t="s">
-        <v>119</v>
-      </c>
-      <c r="B103" t="s">
-        <v>121</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4">
-      <c r="A104" t="s">
-        <v>119</v>
-      </c>
-      <c r="B104" t="s">
-        <v>126</v>
-      </c>
-      <c r="C104" t="s">
-        <v>4</v>
-      </c>
-      <c r="D104" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4">
-      <c r="A106" t="s">
-        <v>125</v>
-      </c>
-      <c r="B106" t="s">
-        <v>126</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4">
-      <c r="A107" t="s">
-        <v>125</v>
-      </c>
-      <c r="B107" t="s">
-        <v>127</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4">
-      <c r="A108" t="s">
-        <v>125</v>
-      </c>
-      <c r="B108" t="s">
-        <v>128</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4">
-      <c r="A109" t="s">
-        <v>125</v>
-      </c>
-      <c r="B109" t="s">
-        <v>146</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="B111" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="B112" t="s">
-        <v>140</v>
+        <v>5</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="B113" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="B114" t="s">
-        <v>139</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4">
-      <c r="A115" t="s">
-        <v>136</v>
-      </c>
-      <c r="B115" t="s">
-        <v>3</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>144</v>
+        <v>125</v>
+      </c>
+      <c r="C114" t="s">
+        <v>4</v>
+      </c>
+      <c r="D114" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="116" spans="1:4">
-      <c r="C116" s="2"/>
-      <c r="D116" s="2"/>
+      <c r="A116" t="s">
+        <v>124</v>
+      </c>
+      <c r="B116" t="s">
+        <v>125</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="B117" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="B118" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>158</v>
+        <v>28</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="B119" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4">
-      <c r="A120" t="s">
-        <v>154</v>
-      </c>
-      <c r="B120" t="s">
-        <v>3</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>159</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" t="s">
+        <v>135</v>
+      </c>
+      <c r="B121" t="s">
+        <v>136</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>171</v>
+        <v>135</v>
       </c>
       <c r="B122" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>173</v>
+        <v>140</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>171</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>71</v>
+        <v>135</v>
+      </c>
+      <c r="B123" t="s">
+        <v>137</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>72</v>
+        <v>142</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
-        <v>171</v>
+        <v>135</v>
       </c>
       <c r="B124" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" t="s">
+        <v>135</v>
+      </c>
+      <c r="B125" t="s">
+        <v>3</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="C126" s="2"/>
+      <c r="D126" s="2"/>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" t="s">
+        <v>153</v>
+      </c>
+      <c r="B127" t="s">
+        <v>159</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" t="s">
+        <v>153</v>
+      </c>
+      <c r="B128" t="s">
+        <v>154</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" t="s">
+        <v>153</v>
+      </c>
+      <c r="B129" t="s">
+        <v>155</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" t="s">
+        <v>153</v>
+      </c>
+      <c r="B130" t="s">
+        <v>3</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" t="s">
+        <v>170</v>
+      </c>
+      <c r="B132" t="s">
         <v>171</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C132" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" t="s">
+        <v>170</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" t="s">
+        <v>170</v>
+      </c>
+      <c r="B134" t="s">
+        <v>166</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" t="s">
+        <v>170</v>
+      </c>
+      <c r="B135" t="s">
         <v>19</v>
       </c>
-      <c r="C125" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4">
-      <c r="A126" t="s">
-        <v>171</v>
-      </c>
-      <c r="B126" t="s">
-        <v>126</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>174</v>
+      <c r="C135" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" t="s">
+        <v>170</v>
+      </c>
+      <c r="B136" t="s">
+        <v>125</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chỉnh lại base và tổ chức thư mục, kéo api department, viết hàm lưu ảnh
</commit_message>
<xml_diff>
--- a/ServiceGeneratorTool/DbSchema.xlsx
+++ b/ServiceGeneratorTool/DbSchema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Restaurant\restaurant-management-api\ServiceGeneratorTool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\School\restaurant-management-api\ServiceGeneratorTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05E3705-428E-434E-9849-7273DEE3EF88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BF5598-D9D3-484D-B880-1E3B91EDFCF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5682C2DE-D9BC-4AE6-9095-A6F08CD2E77F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="220">
   <si>
     <t>TableName</t>
   </si>
@@ -429,9 +429,6 @@
     <t>Nội dung OTP</t>
   </si>
   <si>
-    <t>Mã phòng ban</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -462,15 +459,6 @@
     <t>Giá trị loại hình</t>
   </si>
   <si>
-    <t>DepartmentTypeId</t>
-  </si>
-  <si>
-    <t>Tên phòng ban</t>
-  </si>
-  <si>
-    <t>Loại phòng ban</t>
-  </si>
-  <si>
     <t>ExpiryTime</t>
   </si>
   <si>
@@ -676,6 +664,27 @@
   </si>
   <si>
     <t>Thời điểm gán</t>
+  </si>
+  <si>
+    <t>Mã Cơ sở</t>
+  </si>
+  <si>
+    <t>Tên cơ sở</t>
+  </si>
+  <si>
+    <t>ManagerId</t>
+  </si>
+  <si>
+    <t>Id quản lý</t>
+  </si>
+  <si>
+    <t>int?</t>
+  </si>
+  <si>
+    <t>DepartmentPhoto</t>
+  </si>
+  <si>
+    <t>Ảnh cơ sở</t>
   </si>
 </sst>
 </file>
@@ -1058,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D1BB7ED-A112-494B-BC7C-AC8397CA64F1}">
-  <dimension ref="A1:D148"/>
+  <dimension ref="A1:D149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1223,7 +1232,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>134</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1231,13 +1240,13 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1245,13 +1254,13 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1259,32 +1268,32 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B16" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
@@ -1298,77 +1307,77 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B19" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C19" t="s">
         <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B20" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
+        <v>175</v>
+      </c>
+      <c r="B21" t="s">
         <v>179</v>
-      </c>
-      <c r="B21" t="s">
-        <v>183</v>
       </c>
       <c r="C21" t="s">
         <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B22" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B23" t="s">
         <v>15</v>
@@ -1377,7 +1386,7 @@
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1427,13 +1436,13 @@
         <v>18</v>
       </c>
       <c r="B28" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1447,7 +1456,7 @@
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1455,21 +1464,21 @@
         <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C30" t="s">
         <v>22</v>
       </c>
       <c r="D30" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B32" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -1480,21 +1489,21 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B33" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>9</v>
@@ -1523,7 +1532,7 @@
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1531,7 +1540,7 @@
         <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
@@ -1559,13 +1568,13 @@
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C39" t="s">
         <v>4</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1573,13 +1582,13 @@
         <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C40" t="s">
         <v>22</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1615,7 +1624,7 @@
         <v>21</v>
       </c>
       <c r="B44" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
@@ -1629,13 +1638,13 @@
         <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C45" t="s">
         <v>22</v>
       </c>
       <c r="D45" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1643,13 +1652,13 @@
         <v>21</v>
       </c>
       <c r="B46" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C46" t="s">
         <v>22</v>
       </c>
       <c r="D46" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1657,13 +1666,13 @@
         <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1769,13 +1778,13 @@
         <v>45</v>
       </c>
       <c r="B57" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C57" t="s">
         <v>6</v>
       </c>
       <c r="D57" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1783,13 +1792,13 @@
         <v>45</v>
       </c>
       <c r="B58" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C58" t="s">
         <v>6</v>
       </c>
       <c r="D58" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2091,13 +2100,13 @@
         <v>77</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2517,7 +2526,7 @@
         <v>4</v>
       </c>
       <c r="D119" t="s">
-        <v>134</v>
+        <v>167</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2531,7 +2540,7 @@
         <v>4</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>134</v>
+        <v>213</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2545,7 +2554,7 @@
         <v>6</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>146</v>
+        <v>214</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2567,38 +2576,38 @@
         <v>124</v>
       </c>
       <c r="B124" t="s">
-        <v>145</v>
+        <v>215</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>4</v>
+        <v>217</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4">
-      <c r="A126" t="s">
-        <v>135</v>
-      </c>
-      <c r="B126" t="s">
-        <v>136</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>141</v>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" t="s">
+        <v>124</v>
+      </c>
+      <c r="B125" t="s">
+        <v>218</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" t="s">
+        <v>134</v>
+      </c>
+      <c r="B127" t="s">
         <v>135</v>
       </c>
-      <c r="B127" t="s">
-        <v>139</v>
-      </c>
       <c r="C127" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>140</v>
@@ -2606,38 +2615,38 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B128" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B129" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B130" t="s">
-        <v>3</v>
+        <v>137</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>6</v>
@@ -2647,217 +2656,231 @@
       </c>
     </row>
     <row r="131" spans="1:4">
-      <c r="C131" s="2"/>
-      <c r="D131" s="2"/>
+      <c r="A131" t="s">
+        <v>134</v>
+      </c>
+      <c r="B131" t="s">
+        <v>3</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="132" spans="1:4">
-      <c r="A132" t="s">
-        <v>153</v>
-      </c>
-      <c r="B132" t="s">
-        <v>199</v>
-      </c>
-      <c r="C132" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D132" s="2" t="s">
-        <v>158</v>
-      </c>
+      <c r="C132" s="2"/>
+      <c r="D132" s="2"/>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B133" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B134" t="s">
-        <v>154</v>
+        <v>196</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135" t="s">
+        <v>149</v>
+      </c>
+      <c r="B135" t="s">
+        <v>150</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" t="s">
+        <v>149</v>
+      </c>
+      <c r="B136" t="s">
+        <v>3</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D136" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="B135" t="s">
-        <v>3</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D135" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4">
-      <c r="A137" t="s">
-        <v>168</v>
-      </c>
-      <c r="B137" t="s">
-        <v>169</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D137" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" t="s">
-        <v>168</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>70</v>
+        <v>164</v>
+      </c>
+      <c r="B138" t="s">
+        <v>165</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>71</v>
+        <v>166</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" t="s">
-        <v>168</v>
-      </c>
-      <c r="B139" t="s">
         <v>164</v>
       </c>
+      <c r="B139" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="C139" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>165</v>
+        <v>71</v>
       </c>
     </row>
     <row r="140" spans="1:4">
       <c r="A140" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B140" t="s">
-        <v>19</v>
+        <v>160</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B141" t="s">
+        <v>19</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" t="s">
+        <v>164</v>
+      </c>
+      <c r="B142" t="s">
         <v>125</v>
       </c>
-      <c r="C141" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D141" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4">
-      <c r="A143" t="s">
-        <v>195</v>
-      </c>
-      <c r="B143" t="s">
-        <v>207</v>
-      </c>
-      <c r="C143" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D143" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" ht="15.75" customHeight="1">
+      <c r="C142" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
       <c r="A144" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B144" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C144" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="15.75" customHeight="1">
       <c r="A145" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B145" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="146" spans="1:4">
       <c r="A146" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B146" t="s">
-        <v>197</v>
+        <v>168</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="147" spans="1:4">
       <c r="A147" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B147" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="148" spans="1:4">
       <c r="A148" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B148" t="s">
+        <v>194</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D148" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C148" t="s">
-        <v>6</v>
-      </c>
-      <c r="D148" s="2" t="s">
-        <v>206</v>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" t="s">
+        <v>191</v>
+      </c>
+      <c r="B149" t="s">
+        <v>197</v>
+      </c>
+      <c r="C149" t="s">
+        <v>6</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>